<commit_message>
almost finished with two apps
</commit_message>
<xml_diff>
--- a/locker/BOM_fudlkr.xlsx
+++ b/locker/BOM_fudlkr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2004E3E-C6E9-44BE-ABBA-A4C5B79B0CBD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DA450E-4791-481A-BDD3-918121D822BE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Part #</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Perforated Stainless Steel Metal Sheet (4ftx8ft)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/SODIAL-5-Port-Ethernet-Desktop-Network/dp/B07H9V7HVH/ref=sr_1_cc_4?s=aps&amp;ie=UTF8&amp;qid=1547754841&amp;sr=1-4-catcorr&amp;keywords=hub+network+din</t>
+  </si>
+  <si>
+    <t>Network Unmanaged Switch</t>
   </si>
 </sst>
 </file>
@@ -557,7 +563,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,9 +971,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="E14" s="7" t="s">
         <v>42</v>
       </c>

</xml_diff>